<commit_message>
Website links to curated data files
</commit_message>
<xml_diff>
--- a/tabular/eve/ecv-circo-refseqs-side-data.xlsx
+++ b/tabular/eve/ecv-circo-refseqs-side-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNAss/CRESS-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E39C8C8-6C29-FA45-BB7A-A72DDC687133}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{584CB84A-2F94-BA40-923D-6F37A5794407}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7780" yWindow="1440" windowWidth="41400" windowHeight="15980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7780" yWindow="1440" windowWidth="40260" windowHeight="23420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1484,7 +1484,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Refactoring for DIGS paper update
</commit_message>
<xml_diff>
--- a/tabular/eve/ecv-circo-refseqs-side-data.xlsx
+++ b/tabular/eve/ecv-circo-refseqs-side-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11108"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNAss/CRESS-GLUE/tabular/eve/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/CRESS-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC87EB29-0B82-7D44-8E84-53832CA9ACD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF3754C-9735-454D-9B05-E8FDDF836962}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="460" windowWidth="27840" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21900" yWindow="640" windowWidth="27840" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="187">
   <si>
     <t>Circovirus</t>
   </si>
@@ -416,12 +415,6 @@
     <t>ecv-circo.40-anguilla</t>
   </si>
   <si>
-    <t>ecv-circo.19-anura1</t>
-  </si>
-  <si>
-    <t>ecv-circo.20-anura2</t>
-  </si>
-  <si>
     <t>ecv-circo.21-microcaecilia</t>
   </si>
   <si>
@@ -582,6 +575,24 @@
   </si>
   <si>
     <t>Endogenous circoviral element circo.27.Choloepus</t>
+  </si>
+  <si>
+    <t>ecv-circo.19-anura</t>
+  </si>
+  <si>
+    <t>ecv-circo.20-anura</t>
+  </si>
+  <si>
+    <t>ecv-circo.22-testudines</t>
+  </si>
+  <si>
+    <t>Testudines</t>
+  </si>
+  <si>
+    <t>REF_ECV_Circo-23.Testudines</t>
+  </si>
+  <si>
+    <t>Endogenous circoviral element circo.21-Testiudines reference sequence</t>
   </si>
 </sst>
 </file>
@@ -1938,10 +1949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="A1:M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2214,16 +2225,16 @@
         <v>7</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>25</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>18</v>
@@ -2264,7 +2275,7 @@
         <v>25</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>14</v>
@@ -2305,7 +2316,7 @@
         <v>25</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>29</v>
@@ -2340,13 +2351,13 @@
         <v>115</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>25</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>27</v>
@@ -2381,13 +2392,13 @@
         <v>115</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>25</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>42</v>
@@ -2422,13 +2433,13 @@
         <v>115</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>25</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>49</v>
@@ -2454,25 +2465,25 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B13" s="12">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>115</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>25</v>
+        <v>142</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>32</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>7</v>
@@ -2495,25 +2506,25 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B14" s="12">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>4</v>
+        <v>115</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>25</v>
+        <v>143</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>32</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>7</v>
@@ -2536,25 +2547,25 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>128</v>
+        <v>181</v>
       </c>
       <c r="B15" s="12">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>4</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>25</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>7</v>
@@ -2577,25 +2588,25 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>129</v>
+        <v>182</v>
       </c>
       <c r="B16" s="12">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>115</v>
+        <v>4</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>25</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>7</v>
@@ -2618,25 +2629,25 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B17" s="12">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>115</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>32</v>
+        <v>141</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>7</v>
@@ -2659,25 +2670,25 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>130</v>
+        <v>183</v>
       </c>
       <c r="B18" s="12">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>115</v>
+        <v>4</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>32</v>
+        <v>184</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>165</v>
+        <v>185</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>7</v>
@@ -2700,7 +2711,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B19" s="12">
         <v>25</v>
@@ -2709,16 +2720,16 @@
         <v>115</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E19" s="22" t="s">
         <v>32</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>7</v>
@@ -2741,12 +2752,12 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B20" s="12">
-        <v>30</v>
-      </c>
-      <c r="C20" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>115</v>
       </c>
       <c r="D20" s="15" t="s">
@@ -2756,10 +2767,10 @@
         <v>25</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>7</v>
@@ -2782,25 +2793,25 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="B21" s="12">
-        <v>29</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>4</v>
+        <v>27</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>115</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>25</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>7</v>
@@ -2823,7 +2834,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B22" s="12">
         <v>28</v>
@@ -2832,16 +2843,16 @@
         <v>115</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>25</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>7</v>
@@ -2864,25 +2875,25 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="B23" s="12">
-        <v>26</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>115</v>
+        <v>29</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>4</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>25</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>7</v>
@@ -2905,25 +2916,25 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B24" s="12">
-        <v>27</v>
-      </c>
-      <c r="C24" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="12" t="s">
         <v>115</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>25</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>7</v>
@@ -2944,9 +2955,50 @@
         <v>1</v>
       </c>
     </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B25" s="12">
+        <v>40</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J25" s="3">
+        <v>1</v>
+      </c>
+      <c r="K25" s="3">
+        <v>1</v>
+      </c>
+      <c r="L25" s="3">
+        <v>1</v>
+      </c>
+      <c r="M25" s="3">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M13">
-    <sortCondition ref="B2:B13"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M25">
+    <sortCondition ref="B2:B25"/>
   </sortState>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Refactoring. Cyclocvirus + Circovirus
</commit_message>
<xml_diff>
--- a/tabular/eve/ecv-circo-refseqs-side-data.xlsx
+++ b/tabular/eve/ecv-circo-refseqs-side-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11108"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNAss/CRESS-GLUE/tabular/eve/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/CRESS-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8ECC321-F66C-594A-AC3A-586C7529F9A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB6B4CC-4BAB-2B4C-AAC3-75F92DBECD4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10660" yWindow="3120" windowWidth="27940" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -409,9 +409,6 @@
     <t>ecv-circo.40-anguilla</t>
   </si>
   <si>
-    <t>ecv-circo.21-microcaecilia</t>
-  </si>
-  <si>
     <t>ecv-circo.18-picoides</t>
   </si>
   <si>
@@ -421,12 +418,6 @@
     <t>ecv-circo.30-phascolarctos</t>
   </si>
   <si>
-    <t>ecv-circo.26-manis</t>
-  </si>
-  <si>
-    <t>ecv-circo.27-choloepus</t>
-  </si>
-  <si>
     <t>subclass</t>
   </si>
   <si>
@@ -505,9 +496,6 @@
     <t>REF_ECV_Circo-20.Anura</t>
   </si>
   <si>
-    <t>REF_ECV_Circo-21.Microcaecilia</t>
-  </si>
-  <si>
     <t>REF_ECV_Circo-17.Egretta</t>
   </si>
   <si>
@@ -535,9 +523,6 @@
     <t>Endogenous circoviral element circo.20-Anura reference sequence</t>
   </si>
   <si>
-    <t>Endogenous circoviral element circo.21-Microcaecilia reference sequence</t>
-  </si>
-  <si>
     <t>Endogenous circoviral element circo.17.Egretta</t>
   </si>
   <si>
@@ -565,9 +550,6 @@
     <t>ecv-circo.20-anura</t>
   </si>
   <si>
-    <t>ecv-circo.22-testudines</t>
-  </si>
-  <si>
     <t>Testudines</t>
   </si>
   <si>
@@ -592,12 +574,6 @@
     <t>REF_ECV_Circo-23.Microgale</t>
   </si>
   <si>
-    <t>REF_ECV_Circo-22.Testudines</t>
-  </si>
-  <si>
-    <t>Endogenous circoviral element circo.22-Testudines reference sequence</t>
-  </si>
-  <si>
     <t>Endogenous circoviral element circo.23-Microgale reference sequence</t>
   </si>
   <si>
@@ -620,6 +596,30 @@
   </si>
   <si>
     <t>Endogenous circoviral element circo.28.crocidura</t>
+  </si>
+  <si>
+    <t>ecv-circo.102-testudines</t>
+  </si>
+  <si>
+    <t>REF_ECV_Circo-102.Testudines</t>
+  </si>
+  <si>
+    <t>Endogenous circoviral element circo.102-Testudines reference sequence</t>
+  </si>
+  <si>
+    <t>ecv-circo.27-choloepus-con</t>
+  </si>
+  <si>
+    <t>ecv-circo.26-manis-con</t>
+  </si>
+  <si>
+    <t>ecv-circo.150-microcaecilia</t>
+  </si>
+  <si>
+    <t>Endogenous circoviral element circo.150-Microcaecilia reference sequence</t>
+  </si>
+  <si>
+    <t>REF_ECV_Circo-150.Microcaecilia</t>
   </si>
 </sst>
 </file>
@@ -1979,7 +1979,7 @@
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2211,16 +2211,16 @@
         <v>7</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>25</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>18</v>
@@ -2261,7 +2261,7 @@
         <v>25</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>14</v>
@@ -2302,7 +2302,7 @@
         <v>25</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>29</v>
@@ -2337,13 +2337,13 @@
         <v>113</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>25</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>27</v>
@@ -2378,13 +2378,13 @@
         <v>113</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>25</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>41</v>
@@ -2419,13 +2419,13 @@
         <v>113</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>25</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>48</v>
@@ -2460,16 +2460,16 @@
         <v>113</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E12" s="22" t="s">
         <v>32</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>7</v>
@@ -2492,7 +2492,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B13" s="12">
         <v>18</v>
@@ -2501,16 +2501,16 @@
         <v>113</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E13" s="22" t="s">
         <v>32</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>7</v>
@@ -2533,7 +2533,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B14" s="12">
         <v>19</v>
@@ -2542,16 +2542,16 @@
         <v>4</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>25</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>7</v>
@@ -2574,7 +2574,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B15" s="12">
         <v>20</v>
@@ -2583,16 +2583,16 @@
         <v>4</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>25</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>7</v>
@@ -2615,25 +2615,25 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>125</v>
+        <v>176</v>
       </c>
       <c r="B16" s="12">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>113</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>25</v>
+        <v>178</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>32</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>7</v>
@@ -2659,22 +2659,22 @@
         <v>177</v>
       </c>
       <c r="B17" s="12">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>4</v>
+        <v>113</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>25</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>7</v>
@@ -2697,25 +2697,25 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>182</v>
+        <v>126</v>
       </c>
       <c r="B18" s="12">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>113</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>184</v>
+        <v>138</v>
       </c>
       <c r="E18" s="22" t="s">
         <v>32</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>185</v>
+        <v>156</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>188</v>
+        <v>165</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>7</v>
@@ -2738,25 +2738,25 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="B19" s="12">
-        <v>24</v>
-      </c>
-      <c r="C19" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="14" t="s">
         <v>113</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>179</v>
+        <v>140</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>25</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>7</v>
@@ -2779,25 +2779,25 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>127</v>
+        <v>191</v>
       </c>
       <c r="B20" s="12">
-        <v>25</v>
-      </c>
-      <c r="C20" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>113</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="E20" s="22" t="s">
-        <v>32</v>
+      <c r="E20" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>160</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>7</v>
@@ -2820,25 +2820,25 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>129</v>
+        <v>184</v>
       </c>
       <c r="B21" s="12">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>113</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>143</v>
+        <v>185</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>25</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>163</v>
+        <v>186</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>7</v>
@@ -2861,25 +2861,25 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="B22" s="12">
-        <v>27</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>113</v>
+        <v>29</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>4</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>25</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>7</v>
@@ -2902,25 +2902,25 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>192</v>
+        <v>127</v>
       </c>
       <c r="B23" s="12">
-        <v>28</v>
-      </c>
-      <c r="C23" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="12" t="s">
         <v>113</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>193</v>
+        <v>139</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>25</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>194</v>
+        <v>157</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>195</v>
+        <v>166</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>7</v>
@@ -2943,25 +2943,25 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>145</v>
+        <v>181</v>
       </c>
       <c r="B24" s="12">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>4</v>
+        <v>113</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>25</v>
+        <v>118</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>32</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>162</v>
+        <v>182</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>7</v>
@@ -2984,25 +2984,25 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>128</v>
+        <v>188</v>
       </c>
       <c r="B25" s="12">
-        <v>30</v>
+        <v>102</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>113</v>
+        <v>4</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>142</v>
+        <v>172</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>25</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>161</v>
+        <v>189</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>171</v>
+        <v>190</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>7</v>
@@ -3025,25 +3025,25 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>124</v>
+        <v>193</v>
       </c>
       <c r="B26" s="12">
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>113</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>25</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>153</v>
+        <v>195</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>154</v>
+        <v>194</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>7</v>
@@ -3066,25 +3066,25 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>189</v>
+        <v>124</v>
       </c>
       <c r="B27" s="12">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C27" s="12" t="s">
         <v>113</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="E27" s="22" t="s">
-        <v>32</v>
+        <v>133</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>190</v>
+        <v>150</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>191</v>
+        <v>151</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>7</v>
@@ -3106,8 +3106,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M27">
-    <sortCondition ref="B2:B27"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M24">
+    <sortCondition ref="B2:B24"/>
   </sortState>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3125,10 +3125,13 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD4"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="42.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">

</xml_diff>

<commit_message>
Refactoring numeric IDs of ECVs
</commit_message>
<xml_diff>
--- a/tabular/eve/ecv-circo-refseqs-side-data.xlsx
+++ b/tabular/eve/ecv-circo-refseqs-side-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11108"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNAss/CRESS-GLUE/tabular/eve/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/CRESS-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB477740-79B8-BF4C-BD02-02FA8EC86A48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D9EB2B-38C1-754D-90FA-F99EB977E919}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10660" yWindow="3120" windowWidth="27940" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20600" yWindow="3800" windowWidth="27940" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="141">
   <si>
     <t>Circovirus</t>
   </si>
@@ -55,21 +55,12 @@
     <t>Circoviridae</t>
   </si>
   <si>
-    <t>ecv-circo.11-carnivore-con</t>
-  </si>
-  <si>
-    <t>ecv-circo.5-serpentes-con</t>
-  </si>
-  <si>
     <t>ecv-circo.1-passeriformes-con</t>
   </si>
   <si>
     <t>ecv-circo.2-psittaciformes-con</t>
   </si>
   <si>
-    <t>ecv-circo.7-actinopterygii-con</t>
-  </si>
-  <si>
     <t>REF_ECV_Varroa</t>
   </si>
   <si>
@@ -109,24 +100,15 @@
     <t>Consensus</t>
   </si>
   <si>
-    <t>ecv-circo.13-galeopterus-con</t>
-  </si>
-  <si>
     <t>Endogenous circoviral element circo.13-galeopterus consensus sequence</t>
   </si>
   <si>
-    <t>ecv-circo.12-chrysochloris-con</t>
-  </si>
-  <si>
     <t>Endogenous circoviral element circo.12-chrysochloris consensus sequence</t>
   </si>
   <si>
     <t>numeric_id</t>
   </si>
   <si>
-    <t>ecv-circo.3-mus_caroli</t>
-  </si>
-  <si>
     <t>Reference</t>
   </si>
   <si>
@@ -148,9 +130,6 @@
     <t>Endogenous circoviral element circo.6-cyprinus consensus sequence</t>
   </si>
   <si>
-    <t>ecv-circo.14-tinamou-con</t>
-  </si>
-  <si>
     <t>Endogenous circoviral element circo.14-tinamou consensus sequence</t>
   </si>
   <si>
@@ -184,15 +163,9 @@
     <t>REF_ECV_Circo.3-Mus_caroli</t>
   </si>
   <si>
-    <t>REF_ECV_Circo.5-Serpentes</t>
-  </si>
-  <si>
     <t>REF_ECV_Circo.6-Cyprinus</t>
   </si>
   <si>
-    <t>ecv-circo.15-gallirallus</t>
-  </si>
-  <si>
     <t>order</t>
   </si>
   <si>
@@ -226,21 +199,9 @@
     <t>Chrysochloris_asiatica</t>
   </si>
   <si>
-    <t>ecv-circo.17-egretta</t>
-  </si>
-  <si>
-    <t>ecv-circo.40-anguilla</t>
-  </si>
-  <si>
-    <t>ecv-circo.18-picoides</t>
-  </si>
-  <si>
     <t>ecv-circo.25-heterocephalus</t>
   </si>
   <si>
-    <t>ecv-circo.30-phascolarctos</t>
-  </si>
-  <si>
     <t>subclass</t>
   </si>
   <si>
@@ -283,9 +244,6 @@
     <t>Choloepus</t>
   </si>
   <si>
-    <t>ecv-circo.29-dasyuridae</t>
-  </si>
-  <si>
     <t>Dasyuridae</t>
   </si>
   <si>
@@ -328,12 +286,6 @@
     <t>REF_ECV_Circo-25.Picoides</t>
   </si>
   <si>
-    <t>REF_ECV_Circo-30.Picoides</t>
-  </si>
-  <si>
-    <t>REF_ECV_Circo-29.Dasyuridae</t>
-  </si>
-  <si>
     <t>REF_ECV_Circo-26.Manis</t>
   </si>
   <si>
@@ -358,21 +310,12 @@
     <t>Endogenous circoviral element circo.30.Picoides</t>
   </si>
   <si>
-    <t>Endogenous circoviral element circo.29.Dasyuridae</t>
-  </si>
-  <si>
     <t>Endogenous circoviral element circo.26.Manis</t>
   </si>
   <si>
     <t>Endogenous circoviral element circo.27.Choloepus</t>
   </si>
   <si>
-    <t>ecv-circo.19-anura</t>
-  </si>
-  <si>
-    <t>ecv-circo.20-anura</t>
-  </si>
-  <si>
     <t>Testudines</t>
   </si>
   <si>
@@ -385,33 +328,15 @@
     <t>Endogenous circoviral element circo.24-Sanguinus reference sequence</t>
   </si>
   <si>
-    <t>ecv-circo.23-microgale</t>
-  </si>
-  <si>
-    <t>ecv-circo.24-sanguinus</t>
-  </si>
-  <si>
     <t>Microgale talacazi</t>
   </si>
   <si>
-    <t>REF_ECV_Circo-23.Microgale</t>
-  </si>
-  <si>
-    <t>Endogenous circoviral element circo.23-Microgale reference sequence</t>
-  </si>
-  <si>
-    <t>ecv-circo.44-monodelphis</t>
-  </si>
-  <si>
     <t>REF_ECV_Circo.44-Monodelphis</t>
   </si>
   <si>
     <t>Endogenous circoviral element circo.44-monodelphis domestica reference sequence</t>
   </si>
   <si>
-    <t>ecv-circo.28-crocidura</t>
-  </si>
-  <si>
     <t>Crocidura</t>
   </si>
   <si>
@@ -430,9 +355,6 @@
     <t>Endogenous circoviral element circo.102-Testudines reference sequence</t>
   </si>
   <si>
-    <t>ecv-circo.27-choloepus-con</t>
-  </si>
-  <si>
     <t>ecv-circo.26-manis-con</t>
   </si>
   <si>
@@ -443,6 +365,93 @@
   </si>
   <si>
     <t>REF_ECV_Circo-150.Microcaecilia</t>
+  </si>
+  <si>
+    <t>ecv-circo.105-serpentes-con</t>
+  </si>
+  <si>
+    <t>REF_ECV_Circo.105-Serpentes</t>
+  </si>
+  <si>
+    <t>ecv-circo.104-salvator</t>
+  </si>
+  <si>
+    <t>REF_ECV_Circo.104-Salvator</t>
+  </si>
+  <si>
+    <t>Salvator</t>
+  </si>
+  <si>
+    <t>ecv-circo.51-carnivore-con</t>
+  </si>
+  <si>
+    <t>ecv-circo.52-chrysochloris-con</t>
+  </si>
+  <si>
+    <t>ecv-circo.4-tinamou-con</t>
+  </si>
+  <si>
+    <t>ecv-circo.5-gallirallus</t>
+  </si>
+  <si>
+    <t>ecv-circo.7-egretta</t>
+  </si>
+  <si>
+    <t>ecv-circo.53-mus_caroli</t>
+  </si>
+  <si>
+    <t>ecv-circo.8-picoides</t>
+  </si>
+  <si>
+    <t>ecv-circo.54-sanguinus</t>
+  </si>
+  <si>
+    <t>ecv-circo.57-galeopterus-con</t>
+  </si>
+  <si>
+    <t>ecv-circo.58-crocidura</t>
+  </si>
+  <si>
+    <t>ecv-circo.59-choloepus-con</t>
+  </si>
+  <si>
+    <t>ecv-circo.60-microgale</t>
+  </si>
+  <si>
+    <t>ecv-circo.90-dasyuridae</t>
+  </si>
+  <si>
+    <t>ecv-circo.91-phascolarctos</t>
+  </si>
+  <si>
+    <t>ecv-circo.92-monodelphis</t>
+  </si>
+  <si>
+    <t>ecv-circo.200-actinopterygii-con</t>
+  </si>
+  <si>
+    <t>ecv-circo.240-anguilla</t>
+  </si>
+  <si>
+    <t>REF_ECV_Circo-260.Microgale</t>
+  </si>
+  <si>
+    <t>Endogenous circoviral element circo.60-Microgale reference sequence</t>
+  </si>
+  <si>
+    <t>Endogenous circoviral element circo.90.Dasyuridae</t>
+  </si>
+  <si>
+    <t>REF_ECV_Circo-90.Dasyuridae</t>
+  </si>
+  <si>
+    <t>REF_ECV_circo.91-phascolarctos</t>
+  </si>
+  <si>
+    <t>ecv-circo.151-anura</t>
+  </si>
+  <si>
+    <t>ecv-circo.152-anura</t>
   </si>
 </sst>
 </file>
@@ -510,7 +519,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -541,6 +550,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9948118533890809E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -971,7 +1010,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1002,6 +1041,11 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="418">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1758,10 +1802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1785,16 +1829,16 @@
         <v>5</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
@@ -1812,36 +1856,36 @@
         <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="5">
-        <v>1</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>7</v>
@@ -1863,26 +1907,26 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>11</v>
+      <c r="A3" s="14" t="s">
+        <v>9</v>
       </c>
       <c r="B3" s="5">
         <v>2</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>7</v>
@@ -1904,23 +1948,23 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>31</v>
+      <c r="A4" s="14" t="s">
+        <v>119</v>
       </c>
       <c r="B4" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>32</v>
+        <v>60</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>33</v>
@@ -1945,26 +1989,26 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>9</v>
+      <c r="A5" s="14" t="s">
+        <v>120</v>
       </c>
       <c r="B5" s="5">
         <v>5</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>61</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>7</v>
@@ -1986,26 +2030,26 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>12</v>
+      <c r="A6" s="14" t="s">
+        <v>121</v>
       </c>
       <c r="B6" s="5">
         <v>7</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>25</v>
+        <v>65</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>26</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>18</v>
+        <v>89</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>7</v>
@@ -2027,26 +2071,26 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" s="5">
         <v>8</v>
       </c>
-      <c r="B7" s="5">
-        <v>11</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>54</v>
+      <c r="C7" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>25</v>
+        <v>66</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>26</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>7</v>
@@ -2068,26 +2112,26 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>28</v>
+      <c r="A8" s="18" t="s">
+        <v>117</v>
       </c>
       <c r="B8" s="5">
-        <v>12</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>64</v>
+        <v>51</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>7</v>
@@ -2109,26 +2153,26 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>26</v>
+      <c r="A9" s="18" t="s">
+        <v>118</v>
       </c>
       <c r="B9" s="5">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>72</v>
-      </c>
       <c r="E9" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>7</v>
@@ -2150,26 +2194,26 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>39</v>
+      <c r="A10" s="18" t="s">
+        <v>122</v>
       </c>
       <c r="B10" s="5">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>25</v>
+        <v>50</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>26</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>90</v>
+        <v>43</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>7</v>
@@ -2191,26 +2235,26 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>53</v>
+      <c r="A11" s="18" t="s">
+        <v>124</v>
       </c>
       <c r="B11" s="5">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>47</v>
+        <v>98</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>7</v>
@@ -2232,26 +2276,26 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>65</v>
+      <c r="A12" s="18" t="s">
+        <v>56</v>
       </c>
       <c r="B12" s="5">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>7</v>
@@ -2273,26 +2317,26 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>67</v>
+      <c r="A13" s="18" t="s">
+        <v>108</v>
       </c>
       <c r="B13" s="5">
-        <v>18</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>32</v>
+        <v>69</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>7</v>
@@ -2314,26 +2358,26 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>112</v>
+      <c r="A14" s="18" t="s">
+        <v>125</v>
       </c>
       <c r="B14" s="5">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>103</v>
+        <v>23</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>7</v>
@@ -2355,23 +2399,23 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>113</v>
+      <c r="A15" s="18" t="s">
+        <v>126</v>
       </c>
       <c r="B15" s="5">
-        <v>20</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>4</v>
+        <v>58</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>76</v>
+        <v>102</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>104</v>
@@ -2396,26 +2440,26 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>118</v>
+      <c r="A16" s="18" t="s">
+        <v>127</v>
       </c>
       <c r="B16" s="5">
-        <v>23</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>55</v>
+        <v>59</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>32</v>
+        <v>70</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>121</v>
+        <v>86</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>7</v>
@@ -2437,26 +2481,26 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>119</v>
+      <c r="A17" s="18" t="s">
+        <v>128</v>
       </c>
       <c r="B17" s="5">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>25</v>
+        <v>99</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>26</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>116</v>
+        <v>134</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>7</v>
@@ -2478,26 +2522,26 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>68</v>
+      <c r="A18" s="17" t="s">
+        <v>129</v>
       </c>
       <c r="B18" s="5">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>55</v>
+        <v>4</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>32</v>
+        <v>71</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>98</v>
+        <v>137</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>107</v>
+        <v>136</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>7</v>
@@ -2519,26 +2563,26 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>134</v>
+      <c r="A19" s="17" t="s">
+        <v>130</v>
       </c>
       <c r="B19" s="5">
-        <v>26</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>55</v>
+        <v>91</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>101</v>
+        <v>138</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>7</v>
@@ -2560,26 +2604,26 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>133</v>
+      <c r="A20" s="17" t="s">
+        <v>131</v>
       </c>
       <c r="B20" s="5">
-        <v>27</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>55</v>
+        <v>92</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>25</v>
+        <v>51</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>26</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>7</v>
@@ -2601,26 +2645,26 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>126</v>
+      <c r="A21" s="15" t="s">
+        <v>105</v>
       </c>
       <c r="B21" s="5">
-        <v>28</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>55</v>
+        <v>102</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>4</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>127</v>
+        <v>95</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>7</v>
@@ -2642,26 +2686,26 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>84</v>
+      <c r="A22" s="15" t="s">
+        <v>114</v>
       </c>
       <c r="B22" s="5">
-        <v>29</v>
+        <v>104</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>109</v>
+        <v>12</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>7</v>
@@ -2683,26 +2727,26 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>69</v>
+      <c r="A23" s="15" t="s">
+        <v>112</v>
       </c>
       <c r="B23" s="5">
-        <v>30</v>
+        <v>105</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>108</v>
+        <v>12</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>7</v>
@@ -2724,26 +2768,26 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>123</v>
+      <c r="A24" s="16" t="s">
+        <v>109</v>
       </c>
       <c r="B24" s="5">
-        <v>44</v>
+        <v>150</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>32</v>
+        <v>64</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>7</v>
@@ -2765,26 +2809,26 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>130</v>
+      <c r="A25" s="16" t="s">
+        <v>139</v>
       </c>
       <c r="B25" s="5">
-        <v>102</v>
+        <v>151</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>114</v>
+        <v>63</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>131</v>
+        <v>80</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>132</v>
+        <v>87</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>7</v>
@@ -2806,26 +2850,26 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>135</v>
+      <c r="A26" s="16" t="s">
+        <v>140</v>
       </c>
       <c r="B26" s="5">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>55</v>
+        <v>4</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>137</v>
+        <v>81</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>136</v>
+        <v>88</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>7</v>
@@ -2847,26 +2891,26 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>66</v>
+      <c r="A27" s="13" t="s">
+        <v>132</v>
       </c>
       <c r="B27" s="5">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>93</v>
+        <v>15</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>7</v>
@@ -2887,9 +2931,50 @@
         <v>1</v>
       </c>
     </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="B28" s="5">
+        <v>240</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J28" s="3">
+        <v>1</v>
+      </c>
+      <c r="K28" s="3">
+        <v>1</v>
+      </c>
+      <c r="L28" s="3">
+        <v>1</v>
+      </c>
+      <c r="M28" s="3">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M24">
-    <sortCondition ref="B2:B24"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M28">
+    <sortCondition ref="B2:B28"/>
   </sortState>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2917,22 +3002,22 @@
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B1" s="6">
         <v>100</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>7</v>
@@ -2952,7 +3037,7 @@
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B2" s="5">
         <v>8</v>
@@ -2964,13 +3049,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>7</v>
@@ -2991,7 +3076,7 @@
     </row>
     <row r="3" spans="1:13" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B3" s="6">
         <v>9</v>
@@ -3003,10 +3088,10 @@
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>7</v>
@@ -3026,7 +3111,7 @@
     </row>
     <row r="4" spans="1:13" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B4" s="6">
         <v>10</v>
@@ -3038,13 +3123,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>7</v>
@@ -3064,7 +3149,7 @@
     </row>
     <row r="5" spans="1:13" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B5" s="5">
         <v>6</v>
@@ -3076,13 +3161,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Checked IDs after update
</commit_message>
<xml_diff>
--- a/tabular/eve/ecv-circo-refseqs-side-data.xlsx
+++ b/tabular/eve/ecv-circo-refseqs-side-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNAss/CRESS-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF61CA4-0008-FA45-A9DF-A6D1FC1851C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA4B32D-3D01-0D45-9C6E-B04A7D1BD601}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4280" yWindow="5360" windowWidth="41960" windowHeight="17420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="880" yWindow="580" windowWidth="27920" windowHeight="17420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1646,8 +1646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Set-up ECV reference sequences after consolidating IDs and orthology
</commit_message>
<xml_diff>
--- a/tabular/eve/ecv-circo-refseqs-side-data.xlsx
+++ b/tabular/eve/ecv-circo-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNAss/CRESS-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7499A058-C8F6-DB47-80E2-FB137974D60D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2FE5B1-2920-7247-BF1A-CA2DD0FCA82D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14800" yWindow="2720" windowWidth="29640" windowHeight="24020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1683,7 +1683,7 @@
   <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Refactor ECV component - update to latest DIGS iteration
</commit_message>
<xml_diff>
--- a/tabular/eve/ecv-circo-refseqs-side-data.xlsx
+++ b/tabular/eve/ecv-circo-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNAss/CRESS-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D63722E-792A-264C-B360-0BF0D6DCF4A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B188C5C6-7E87-FE4A-B475-8C380885B131}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14800" yWindow="2720" windowWidth="29640" windowHeight="24020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="104">
   <si>
     <t>Circovirus</t>
   </si>
@@ -338,6 +338,9 @@
   </si>
   <si>
     <t>ecv-circo.151-anura-con</t>
+  </si>
+  <si>
+    <t>ecv-circo.150-microcaecilia-con</t>
   </si>
 </sst>
 </file>
@@ -1683,7 +1686,7 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2894,7 +2897,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>63</v>
+        <v>103</v>
       </c>
       <c r="B30" s="20">
         <v>150</v>

</xml_diff>

<commit_message>
Added new CRESS EVEs
</commit_message>
<xml_diff>
--- a/tabular/eve/ecv-circo-refseqs-side-data.xlsx
+++ b/tabular/eve/ecv-circo-refseqs-side-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11213"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNAss/CRESS-GLUE/tabular/eve/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/CRESS-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DAC3D85-24CF-7E47-819C-33F8880A4A27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FBB6E30-C0E8-9149-94E7-D5A3570F7FC3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14800" yWindow="2720" windowWidth="29640" windowHeight="24020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="120">
   <si>
     <t>Circovirus</t>
   </si>
@@ -350,6 +350,45 @@
   </si>
   <si>
     <t>ecv-circo.102-testudines-con</t>
+  </si>
+  <si>
+    <t>ecv-circo.207-parambassis-ranga</t>
+  </si>
+  <si>
+    <t>Parambassis ranga</t>
+  </si>
+  <si>
+    <t>ecv-circo.208-chaenocephalus</t>
+  </si>
+  <si>
+    <t>Chaenocephalus aceratus</t>
+  </si>
+  <si>
+    <t>host_class</t>
+  </si>
+  <si>
+    <t>aves</t>
+  </si>
+  <si>
+    <t>marsupialia</t>
+  </si>
+  <si>
+    <t>boreoeutheria</t>
+  </si>
+  <si>
+    <t>reptile</t>
+  </si>
+  <si>
+    <t>amphibia</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>remove</t>
+  </si>
+  <si>
+    <t>fish</t>
   </si>
 </sst>
 </file>
@@ -404,7 +443,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -459,6 +498,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14996795556505021"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -889,7 +940,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -934,6 +985,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1692,30 +1750,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.83203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15" style="6" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="35" style="2" customWidth="1"/>
-    <col min="7" max="7" width="85.33203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="15.5" style="2" customWidth="1"/>
-    <col min="9" max="9" width="13.83203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" style="6" customWidth="1"/>
-    <col min="11" max="11" width="15.83203125" style="6" customWidth="1"/>
-    <col min="12" max="13" width="10.83203125" style="6"/>
-    <col min="14" max="16384" width="10.83203125" style="2"/>
+    <col min="2" max="4" width="15" style="6" customWidth="1"/>
+    <col min="5" max="5" width="24.1640625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="35" style="2" customWidth="1"/>
+    <col min="9" max="9" width="85.33203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="15.5" style="2" customWidth="1"/>
+    <col min="11" max="11" width="13.83203125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="9.6640625" style="6" customWidth="1"/>
+    <col min="13" max="13" width="15.83203125" style="6" customWidth="1"/>
+    <col min="14" max="15" width="10.83203125" style="6"/>
+    <col min="16" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1723,482 +1781,526 @@
         <v>18</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="20">
+        <v>150</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="5">
+        <v>1</v>
+      </c>
+      <c r="M2" s="5">
+        <v>1</v>
+      </c>
+      <c r="N2" s="5">
+        <v>1</v>
+      </c>
+      <c r="O2" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="20">
+        <v>151</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L3" s="5">
+        <v>1</v>
+      </c>
+      <c r="M3" s="5">
+        <v>1</v>
+      </c>
+      <c r="N3" s="5">
+        <v>1</v>
+      </c>
+      <c r="O3" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="16">
-        <v>1</v>
-      </c>
-      <c r="C2" s="11" t="s">
+      <c r="B4" s="16">
+        <v>1</v>
+      </c>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="F4" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="G4" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="H4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="I4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="5">
-        <v>1</v>
-      </c>
-      <c r="K2" s="5">
-        <v>1</v>
-      </c>
-      <c r="L2" s="5">
-        <v>1</v>
-      </c>
-      <c r="M2" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="J4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4" s="5">
+        <v>1</v>
+      </c>
+      <c r="M4" s="5">
+        <v>1</v>
+      </c>
+      <c r="N4" s="5">
+        <v>1</v>
+      </c>
+      <c r="O4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B5" s="16">
         <v>2</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C5" s="16"/>
+      <c r="D5" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="F5" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="G5" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="H5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="I5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J3" s="5">
-        <v>1</v>
-      </c>
-      <c r="K3" s="5">
-        <v>1</v>
-      </c>
-      <c r="L3" s="5">
-        <v>1</v>
-      </c>
-      <c r="M3" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="J5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L5" s="5">
+        <v>1</v>
+      </c>
+      <c r="M5" s="5">
+        <v>1</v>
+      </c>
+      <c r="N5" s="5">
+        <v>1</v>
+      </c>
+      <c r="O5" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B6" s="16">
         <v>4</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C6" s="16"/>
+      <c r="D6" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="F6" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="G6" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="H6" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="I6" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J4" s="5">
-        <v>1</v>
-      </c>
-      <c r="K4" s="5">
-        <v>1</v>
-      </c>
-      <c r="L4" s="5">
-        <v>1</v>
-      </c>
-      <c r="M4" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="J6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L6" s="5">
+        <v>1</v>
+      </c>
+      <c r="M6" s="5">
+        <v>1</v>
+      </c>
+      <c r="N6" s="5">
+        <v>1</v>
+      </c>
+      <c r="O6" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B7" s="16">
         <v>5</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C7" s="16"/>
+      <c r="D7" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E7" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="F7" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="G7" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="H7" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="I7" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J5" s="5">
-        <v>1</v>
-      </c>
-      <c r="K5" s="5">
-        <v>1</v>
-      </c>
-      <c r="L5" s="5">
-        <v>1</v>
-      </c>
-      <c r="M5" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="J7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L7" s="5">
+        <v>1</v>
+      </c>
+      <c r="M7" s="5">
+        <v>1</v>
+      </c>
+      <c r="N7" s="5">
+        <v>1</v>
+      </c>
+      <c r="O7" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B6" s="16">
-        <v>7</v>
-      </c>
-      <c r="C6" s="11" t="s">
+      <c r="B8" s="16">
+        <v>7</v>
+      </c>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="F8" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="G8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="H8" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="I8" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J6" s="5">
-        <v>1</v>
-      </c>
-      <c r="K6" s="5">
-        <v>1</v>
-      </c>
-      <c r="L6" s="5">
-        <v>1</v>
-      </c>
-      <c r="M6" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="J8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L8" s="5">
+        <v>1</v>
+      </c>
+      <c r="M8" s="5">
+        <v>1</v>
+      </c>
+      <c r="N8" s="5">
+        <v>1</v>
+      </c>
+      <c r="O8" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B9" s="16">
         <v>8</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C9" s="16"/>
+      <c r="D9" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="F9" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="G9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="H9" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="I9" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J7" s="5">
-        <v>1</v>
-      </c>
-      <c r="K7" s="5">
-        <v>1</v>
-      </c>
-      <c r="L7" s="5">
-        <v>1</v>
-      </c>
-      <c r="M7" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="J9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L9" s="5">
+        <v>1</v>
+      </c>
+      <c r="M9" s="5">
+        <v>1</v>
+      </c>
+      <c r="N9" s="5">
+        <v>1</v>
+      </c>
+      <c r="O9" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B10" s="17">
         <v>51</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C10" s="17"/>
+      <c r="D10" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E10" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="F10" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="G10" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="H10" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="I10" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J8" s="5">
-        <v>1</v>
-      </c>
-      <c r="K8" s="5">
-        <v>1</v>
-      </c>
-      <c r="L8" s="5">
-        <v>1</v>
-      </c>
-      <c r="M8" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="J10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L10" s="5">
+        <v>1</v>
+      </c>
+      <c r="M10" s="5">
+        <v>1</v>
+      </c>
+      <c r="N10" s="5">
+        <v>1</v>
+      </c>
+      <c r="O10" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B11" s="17">
         <v>52</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C11" s="17"/>
+      <c r="D11" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E11" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="F11" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="G11" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="H11" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="I11" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J9" s="5">
-        <v>1</v>
-      </c>
-      <c r="K9" s="5">
-        <v>1</v>
-      </c>
-      <c r="L9" s="5">
-        <v>1</v>
-      </c>
-      <c r="M9" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="B10" s="17">
-        <v>53</v>
-      </c>
-      <c r="C10" s="15" t="s">
+      <c r="J11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L11" s="5">
+        <v>1</v>
+      </c>
+      <c r="M11" s="5">
+        <v>1</v>
+      </c>
+      <c r="N11" s="5">
+        <v>1</v>
+      </c>
+      <c r="O11" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="B12" s="17">
+        <v>54</v>
+      </c>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E12" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J10" s="5">
-        <v>1</v>
-      </c>
-      <c r="K10" s="5">
-        <v>1</v>
-      </c>
-      <c r="L10" s="5">
-        <v>1</v>
-      </c>
-      <c r="M10" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="B11" s="17">
-        <v>54</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="15" t="s">
+      <c r="F12" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="G12" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="H12" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="I12" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J11" s="5">
-        <v>1</v>
-      </c>
-      <c r="K11" s="5">
-        <v>1</v>
-      </c>
-      <c r="L11" s="5">
-        <v>1</v>
-      </c>
-      <c r="M11" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="B12" s="17">
-        <v>55</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J12" s="5">
-        <v>1</v>
-      </c>
-      <c r="K12" s="5">
-        <v>1</v>
+      <c r="J12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>0</v>
       </c>
       <c r="L12" s="5">
         <v>1</v>
@@ -2206,40 +2308,44 @@
       <c r="M12" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12" s="5">
+        <v>1</v>
+      </c>
+      <c r="O12" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>85</v>
       </c>
       <c r="B13" s="17">
         <v>56</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="17"/>
+      <c r="D13" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E13" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="F13" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="G13" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="H13" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="G13" s="15" t="s">
+      <c r="I13" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="H13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J13" s="5">
-        <v>1</v>
-      </c>
-      <c r="K13" s="5">
-        <v>1</v>
+      <c r="J13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>0</v>
       </c>
       <c r="L13" s="5">
         <v>1</v>
@@ -2247,40 +2353,44 @@
       <c r="M13" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N13" s="5">
+        <v>1</v>
+      </c>
+      <c r="O13" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>75</v>
       </c>
       <c r="B14" s="17">
         <v>57</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="17"/>
+      <c r="D14" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E14" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="F14" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="G14" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="15" t="s">
+      <c r="H14" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="I14" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J14" s="5">
-        <v>1</v>
-      </c>
-      <c r="K14" s="5">
-        <v>1</v>
+      <c r="J14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>0</v>
       </c>
       <c r="L14" s="5">
         <v>1</v>
@@ -2288,40 +2398,44 @@
       <c r="M14" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N14" s="5">
+        <v>1</v>
+      </c>
+      <c r="O14" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>76</v>
       </c>
       <c r="B15" s="17">
         <v>58</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="17"/>
+      <c r="D15" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E15" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="F15" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="G15" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="H15" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="G15" s="15" t="s">
+      <c r="I15" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="H15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J15" s="5">
-        <v>1</v>
-      </c>
-      <c r="K15" s="5">
-        <v>1</v>
+      <c r="J15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>0</v>
       </c>
       <c r="L15" s="5">
         <v>1</v>
@@ -2329,40 +2443,44 @@
       <c r="M15" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15" s="5">
+        <v>1</v>
+      </c>
+      <c r="O15" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>77</v>
       </c>
       <c r="B16" s="17">
         <v>59</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="17"/>
+      <c r="D16" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E16" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="F16" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="G16" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="H16" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="G16" s="15" t="s">
+      <c r="I16" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J16" s="5">
-        <v>1</v>
-      </c>
-      <c r="K16" s="5">
-        <v>1</v>
+      <c r="J16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>0</v>
       </c>
       <c r="L16" s="5">
         <v>1</v>
@@ -2370,748 +2488,918 @@
       <c r="M16" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16" s="5">
+        <v>1</v>
+      </c>
+      <c r="O16" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="17">
+        <v>62</v>
+      </c>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L17" s="5">
+        <v>1</v>
+      </c>
+      <c r="M17" s="5">
+        <v>1</v>
+      </c>
+      <c r="N17" s="5">
+        <v>1</v>
+      </c>
+      <c r="O17" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B18" s="17">
+        <v>64</v>
+      </c>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L18" s="5">
+        <v>1</v>
+      </c>
+      <c r="M18" s="5">
+        <v>1</v>
+      </c>
+      <c r="N18" s="5">
+        <v>1</v>
+      </c>
+      <c r="O18" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="17">
+        <v>53</v>
+      </c>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L19" s="5">
+        <v>1</v>
+      </c>
+      <c r="M19" s="5">
+        <v>1</v>
+      </c>
+      <c r="N19" s="5">
+        <v>1</v>
+      </c>
+      <c r="O19" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" s="17">
+        <v>55</v>
+      </c>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="I20" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L20" s="5">
+        <v>1</v>
+      </c>
+      <c r="M20" s="5">
+        <v>1</v>
+      </c>
+      <c r="N20" s="5">
+        <v>1</v>
+      </c>
+      <c r="O20" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="17">
+      <c r="B21" s="17">
         <v>60</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C21" s="17"/>
+      <c r="D21" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E21" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="F21" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="G21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="15" t="s">
+      <c r="H21" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="G17" s="15" t="s">
+      <c r="I21" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="H17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J17" s="5">
-        <v>1</v>
-      </c>
-      <c r="K17" s="5">
-        <v>1</v>
-      </c>
-      <c r="L17" s="5">
-        <v>1</v>
-      </c>
-      <c r="M17" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
+      <c r="J21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L21" s="5">
+        <v>1</v>
+      </c>
+      <c r="M21" s="5">
+        <v>1</v>
+      </c>
+      <c r="N21" s="5">
+        <v>1</v>
+      </c>
+      <c r="O21" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="B18" s="17">
+      <c r="B22" s="17">
         <v>61</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C22" s="17"/>
+      <c r="D22" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E22" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="F22" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="G22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="H22" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="G18" s="15" t="s">
+      <c r="I22" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="H18" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J18" s="5">
-        <v>1</v>
-      </c>
-      <c r="K18" s="5">
-        <v>1</v>
-      </c>
-      <c r="L18" s="5">
-        <v>1</v>
-      </c>
-      <c r="M18" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
+      <c r="J22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L22" s="5">
+        <v>1</v>
+      </c>
+      <c r="M22" s="5">
+        <v>1</v>
+      </c>
+      <c r="N22" s="5">
+        <v>1</v>
+      </c>
+      <c r="O22" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" s="17">
+        <v>63</v>
+      </c>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H23" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="I23" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L23" s="5">
+        <v>1</v>
+      </c>
+      <c r="M23" s="5">
+        <v>1</v>
+      </c>
+      <c r="N23" s="5">
+        <v>1</v>
+      </c>
+      <c r="O23" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" s="17">
+        <v>65</v>
+      </c>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="I24" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L24" s="5">
+        <v>1</v>
+      </c>
+      <c r="M24" s="5">
+        <v>1</v>
+      </c>
+      <c r="N24" s="5">
+        <v>1</v>
+      </c>
+      <c r="O24" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" s="17">
+        <v>66</v>
+      </c>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H25" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="I25" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L25" s="5">
+        <v>1</v>
+      </c>
+      <c r="M25" s="5">
+        <v>1</v>
+      </c>
+      <c r="N25" s="5">
+        <v>1</v>
+      </c>
+      <c r="O25" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" s="21">
+        <v>200</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G26" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L26" s="5">
+        <v>1</v>
+      </c>
+      <c r="M26" s="5">
+        <v>1</v>
+      </c>
+      <c r="N26" s="5">
+        <v>1</v>
+      </c>
+      <c r="O26" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" s="21">
+        <v>240</v>
+      </c>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G27" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="I27" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L27" s="5">
+        <v>1</v>
+      </c>
+      <c r="M27" s="5">
+        <v>1</v>
+      </c>
+      <c r="N27" s="5">
+        <v>1</v>
+      </c>
+      <c r="O27" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" s="21">
+        <v>206</v>
+      </c>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="I28" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L28" s="5">
+        <v>1</v>
+      </c>
+      <c r="M28" s="5">
+        <v>1</v>
+      </c>
+      <c r="N28" s="5">
+        <v>1</v>
+      </c>
+      <c r="O28" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B29" s="21">
+        <v>207</v>
+      </c>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L29" s="5">
+        <v>1</v>
+      </c>
+      <c r="M29" s="5">
+        <v>1</v>
+      </c>
+      <c r="N29" s="5">
+        <v>1</v>
+      </c>
+      <c r="O29" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B30" s="21">
+        <v>208</v>
+      </c>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="F30" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H30" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="I30" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L30" s="5">
+        <v>1</v>
+      </c>
+      <c r="M30" s="5">
+        <v>1</v>
+      </c>
+      <c r="N30" s="5">
+        <v>1</v>
+      </c>
+      <c r="O30" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" s="18">
+        <v>90</v>
+      </c>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="G31" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H31" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="I31" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L31" s="5">
+        <v>1</v>
+      </c>
+      <c r="M31" s="5">
+        <v>1</v>
+      </c>
+      <c r="N31" s="5">
+        <v>1</v>
+      </c>
+      <c r="O31" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" s="18">
+        <v>91</v>
+      </c>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="G32" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="I32" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L32" s="5">
+        <v>1</v>
+      </c>
+      <c r="M32" s="5">
+        <v>1</v>
+      </c>
+      <c r="N32" s="5">
+        <v>1</v>
+      </c>
+      <c r="O32" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33" s="18">
         <v>92</v>
       </c>
-      <c r="B19" s="17">
+      <c r="C33" s="18"/>
+      <c r="D33" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H33" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="I33" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L33" s="5">
+        <v>1</v>
+      </c>
+      <c r="M33" s="5">
+        <v>1</v>
+      </c>
+      <c r="N33" s="5">
+        <v>1</v>
+      </c>
+      <c r="O33" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B34" s="19">
+        <v>102</v>
+      </c>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G34" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H34" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="I34" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L34" s="5">
+        <v>1</v>
+      </c>
+      <c r="M34" s="5">
+        <v>1</v>
+      </c>
+      <c r="N34" s="5">
+        <v>1</v>
+      </c>
+      <c r="O34" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" s="19">
+        <v>104</v>
+      </c>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="E35" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" s="3" t="s">
+      <c r="F35" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="G35" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F19" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="G19" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J19" s="5">
-        <v>1</v>
-      </c>
-      <c r="K19" s="5">
-        <v>1</v>
-      </c>
-      <c r="L19" s="5">
-        <v>1</v>
-      </c>
-      <c r="M19" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="B20" s="17">
-        <v>63</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="G20" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J20" s="5">
-        <v>1</v>
-      </c>
-      <c r="K20" s="5">
-        <v>1</v>
-      </c>
-      <c r="L20" s="5">
-        <v>1</v>
-      </c>
-      <c r="M20" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
+      <c r="H35" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="I35" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L35" s="5">
+        <v>1</v>
+      </c>
+      <c r="M35" s="5">
+        <v>1</v>
+      </c>
+      <c r="N35" s="5">
+        <v>1</v>
+      </c>
+      <c r="O35" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="19">
         <v>105</v>
       </c>
-      <c r="B21" s="17">
+      <c r="C36" s="19"/>
+      <c r="D36" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G36" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H36" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C21" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="G21" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J21" s="5">
-        <v>1</v>
-      </c>
-      <c r="K21" s="5">
-        <v>1</v>
-      </c>
-      <c r="L21" s="5">
-        <v>1</v>
-      </c>
-      <c r="M21" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="B22" s="17">
-        <v>65</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="G22" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J22" s="5">
-        <v>1</v>
-      </c>
-      <c r="K22" s="5">
-        <v>1</v>
-      </c>
-      <c r="L22" s="5">
-        <v>1</v>
-      </c>
-      <c r="M22" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="B23" s="17">
-        <v>66</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F23" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="G23" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J23" s="5">
-        <v>1</v>
-      </c>
-      <c r="K23" s="5">
-        <v>1</v>
-      </c>
-      <c r="L23" s="5">
-        <v>1</v>
-      </c>
-      <c r="M23" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="B24" s="18">
-        <v>90</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="G24" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J24" s="5">
-        <v>1</v>
-      </c>
-      <c r="K24" s="5">
-        <v>1</v>
-      </c>
-      <c r="L24" s="5">
-        <v>1</v>
-      </c>
-      <c r="M24" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="B25" s="18">
-        <v>91</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="G25" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J25" s="5">
-        <v>1</v>
-      </c>
-      <c r="K25" s="5">
-        <v>1</v>
-      </c>
-      <c r="L25" s="5">
-        <v>1</v>
-      </c>
-      <c r="M25" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B26" s="18">
-        <v>92</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="G26" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J26" s="5">
-        <v>1</v>
-      </c>
-      <c r="K26" s="5">
-        <v>1</v>
-      </c>
-      <c r="L26" s="5">
-        <v>1</v>
-      </c>
-      <c r="M26" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="B27" s="19">
-        <v>102</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J27" s="5">
-        <v>1</v>
-      </c>
-      <c r="K27" s="5">
-        <v>1</v>
-      </c>
-      <c r="L27" s="5">
-        <v>1</v>
-      </c>
-      <c r="M27" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B28" s="19">
-        <v>104</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J28" s="5">
-        <v>1</v>
-      </c>
-      <c r="K28" s="5">
-        <v>1</v>
-      </c>
-      <c r="L28" s="5">
-        <v>1</v>
-      </c>
-      <c r="M28" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="12" t="s">
+      <c r="I36" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="19">
-        <v>105</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J29" s="5">
-        <v>1</v>
-      </c>
-      <c r="K29" s="5">
-        <v>1</v>
-      </c>
-      <c r="L29" s="5">
-        <v>1</v>
-      </c>
-      <c r="M29" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="B30" s="20">
-        <v>150</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F30" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="G30" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J30" s="5">
-        <v>1</v>
-      </c>
-      <c r="K30" s="5">
-        <v>1</v>
-      </c>
-      <c r="L30" s="5">
-        <v>1</v>
-      </c>
-      <c r="M30" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="B31" s="20">
-        <v>151</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F31" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="G31" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I31" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J31" s="5">
-        <v>1</v>
-      </c>
-      <c r="K31" s="5">
-        <v>1</v>
-      </c>
-      <c r="L31" s="5">
-        <v>1</v>
-      </c>
-      <c r="M31" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="B32" s="21">
-        <v>200</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F32" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="G32" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J32" s="5">
-        <v>1</v>
-      </c>
-      <c r="K32" s="5">
-        <v>1</v>
-      </c>
-      <c r="L32" s="5">
-        <v>1</v>
-      </c>
-      <c r="M32" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="B33" s="21">
-        <v>240</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F33" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="G33" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J33" s="5">
-        <v>1</v>
-      </c>
-      <c r="K33" s="5">
-        <v>1</v>
-      </c>
-      <c r="L33" s="5">
-        <v>1</v>
-      </c>
-      <c r="M33" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="B34" s="21">
-        <v>206</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F34" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="G34" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J34" s="5">
-        <v>1</v>
-      </c>
-      <c r="K34" s="5">
-        <v>1</v>
-      </c>
-      <c r="L34" s="5">
-        <v>1</v>
-      </c>
-      <c r="M34" s="5">
+      <c r="J36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L36" s="5">
+        <v>1</v>
+      </c>
+      <c r="M36" s="5">
+        <v>1</v>
+      </c>
+      <c r="N36" s="5">
+        <v>1</v>
+      </c>
+      <c r="O36" s="5">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M33">
-    <sortCondition ref="B2:B33"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O36">
+    <sortCondition ref="D2:D36"/>
   </sortState>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>